<commit_message>
prettier, and with backup files
</commit_message>
<xml_diff>
--- a/app/docs/templates/qa.xlsx
+++ b/app/docs/templates/qa.xlsx
@@ -24,12 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>Q</t>
   </si>
   <si>
     <t>the long, multi part question that might need several lines.   Q lines will be ignored when importing the answers into the report doc.</t>
@@ -408,7 +405,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -420,21 +417,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -442,11 +436,11 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -454,11 +448,11 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -466,19 +460,16 @@
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
         <v>1</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -486,11 +477,11 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -498,11 +489,11 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -510,16 +501,16 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>